<commit_message>
Updated questions and topics.
</commit_message>
<xml_diff>
--- a/salesforce/Interview Questions April 2021.xlsx
+++ b/salesforce/Interview Questions April 2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanketvaidya/RZume/salesforce/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\•Sanket\GitRepos\Resume\salesforce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2DB1ED-D006-8143-82E1-960E00C14B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A16FE0-F0E1-4137-892B-ECA6BF2B9021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -61,14 +61,6 @@
   </si>
   <si>
     <t>What do you mean by governor limits?</t>
-  </si>
-  <si>
-    <t>Governor limits control how much data can be stored on a shared database. They help to ensure that no one monopolizes the shared resources (Storage, CPU, Memory).
-Here are some few examples of governor limits in Salesforce:
-Maximum CPU time on the Salesforce servers - 10,000ms 
-Total number of sendEmail methods allowed - 10
-Total number of records retrieved by a SOQL query - 50,000 
-Total number of callouts in a transaction - 100</t>
   </si>
   <si>
     <t>What are some things that you can do to prevent governor limits?</t>
@@ -288,12 +280,30 @@
   <si>
     <t>Difference between Stateful and Stateless</t>
   </si>
+  <si>
+    <t>They help to ensure that no one monopolizes the shared resources (Storage, CPU, Memory).
+Here are some few examples of governor limits in Salesforce:
+Maximum CPU time on the Salesforce servers - 10,000ms 
+Total number of sendEmail methods allowed - 10
+Total number of records retrieved by a SOQL query - 50,000 
+Total number of callouts in a transaction - 100</t>
+  </si>
+  <si>
+    <t>•Custom metadata does not support hierarchy type of data based on user profile or a specific user.
+•Custom settings data cannot be deployed using packages or metadata API/Change Sets.
+•Custom settings do not support relationship fields.
+•Custom setting data is not visible in test classes whereas metadata types are visible in test class without the “SeeAllData” annotation.
+•Custom metadata records are deployable and packageable, but Custom setting data is not.</t>
+  </si>
+  <si>
+    <t>https://sfdcgenius.com/difference-between-custom-settings-and-custom-metadata-types/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,6 +335,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF4A4A4A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -375,10 +393,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -403,8 +422,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -427,13 +450,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>31750</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>54390</xdr:rowOff>
+      <xdr:rowOff>54389</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1818428</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1011206</xdr:rowOff>
+      <xdr:colOff>2564423</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>156746</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -456,8 +479,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6119813" y="6721890"/>
-          <a:ext cx="1786678" cy="1248916"/>
+          <a:off x="6113096" y="7293389"/>
+          <a:ext cx="2532673" cy="1626357"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -732,333 +755,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DEC8F1-8C56-49CA-B706-5FDD17539594}">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="74.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="74.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="74.5" style="3"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="74.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="C15" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="3" t="s">
-        <v>31</v>
+      <c r="B18" t="s">
+        <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="256" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="B40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B62" s="11"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B80" s="3"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="11"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C15" r:id="rId1" xr:uid="{42F78AF6-C8A6-4CCC-AD8B-99DD242CC004}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Internal to Wipro</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1070,18 +1105,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="47.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="47.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1092,25 +1127,25 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1140,10 +1175,10 @@
         <v>4.333333333333333</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1152,10 +1187,10 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
     </row>
   </sheetData>

</xml_diff>